<commit_message>
main.py: added parameters to_dict and properties added
</commit_message>
<xml_diff>
--- a/files/reports/2021-10-27/resources-report.xlsx
+++ b/files/reports/2021-10-27/resources-report.xlsx
@@ -40,223 +40,223 @@
     <t>Percentage</t>
   </si>
   <si>
+    <t>Skill Summary - 1</t>
+  </si>
+  <si>
+    <t>Orirock</t>
+  </si>
+  <si>
+    <t>Skill Summary - 2</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>Polyester</t>
+  </si>
+  <si>
+    <t>RMA70-12</t>
+  </si>
+  <si>
+    <t>Skill Summary - 3</t>
+  </si>
+  <si>
+    <t>Orirock Cluster</t>
+  </si>
+  <si>
+    <t>Oriron Shard</t>
+  </si>
+  <si>
+    <t>Polyketon</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Polyester Pack</t>
+  </si>
+  <si>
+    <t>Oriron Cluster</t>
+  </si>
+  <si>
+    <t>Diketon</t>
+  </si>
+  <si>
+    <t>Orirock Cube</t>
+  </si>
+  <si>
+    <t>Manganese Ore</t>
+  </si>
+  <si>
+    <t>Grindstone</t>
+  </si>
+  <si>
+    <t>Loxic Kohl</t>
+  </si>
+  <si>
+    <t>Ester</t>
+  </si>
+  <si>
+    <t>Oriron</t>
+  </si>
+  <si>
     <t>Aketon</t>
   </si>
   <si>
+    <t>Sugar Pack</t>
+  </si>
+  <si>
+    <t>Damaged Device</t>
+  </si>
+  <si>
+    <t>Sugar Substitute</t>
+  </si>
+  <si>
+    <t>Integrated Device</t>
+  </si>
+  <si>
+    <t>Coagulating Gel</t>
+  </si>
+  <si>
+    <t>Sniper Chip</t>
+  </si>
+  <si>
+    <t>Sniper Chip Pack</t>
+  </si>
+  <si>
+    <t>Grindstone Pentahydrate</t>
+  </si>
+  <si>
+    <t>Keton Colloid</t>
+  </si>
+  <si>
+    <t>Polymerized Gel</t>
+  </si>
+  <si>
     <t>Bipolar Nanoflake</t>
   </si>
   <si>
+    <t>White Horse Kohl</t>
+  </si>
+  <si>
+    <t>Incandescent Alloy Block</t>
+  </si>
+  <si>
+    <t>RMA70-24</t>
+  </si>
+  <si>
+    <t>Orirock Concentration</t>
+  </si>
+  <si>
+    <t>Incandescent Alloy</t>
+  </si>
+  <si>
+    <t>Manganese Trihydrate</t>
+  </si>
+  <si>
+    <t>Polymerization Preparation</t>
+  </si>
+  <si>
+    <t>D32 Steel</t>
+  </si>
+  <si>
+    <t>Oriron Block</t>
+  </si>
+  <si>
+    <t>Guard Chip</t>
+  </si>
+  <si>
+    <t>Guard Chip Pack</t>
+  </si>
+  <si>
+    <t>Vanguard Chip</t>
+  </si>
+  <si>
+    <t>Vanguard Chip Pack</t>
+  </si>
+  <si>
+    <t>Crystalline Electroassembly</t>
+  </si>
+  <si>
+    <t>Defender Chip</t>
+  </si>
+  <si>
+    <t>Defender Chip Pack</t>
+  </si>
+  <si>
+    <t>Optimized Device</t>
+  </si>
+  <si>
     <t>Caster Chip</t>
   </si>
   <si>
     <t>Caster Chip Pack</t>
   </si>
   <si>
+    <t>Polyester Lump</t>
+  </si>
+  <si>
+    <t>Sugar Lump</t>
+  </si>
+  <si>
+    <t>Supporter Chip</t>
+  </si>
+  <si>
+    <t>Supporter Chip Pack</t>
+  </si>
+  <si>
+    <t>Specialist Chip</t>
+  </si>
+  <si>
+    <t>Specialist Chip Pack</t>
+  </si>
+  <si>
+    <t>Medic Chip</t>
+  </si>
+  <si>
+    <t>Medic Chip Pack</t>
+  </si>
+  <si>
+    <t>Crystalline Component</t>
+  </si>
+  <si>
+    <t>Crystalline Circuit</t>
+  </si>
+  <si>
+    <t>Semi-natural Solvent</t>
+  </si>
+  <si>
+    <t>Refined Solvent</t>
+  </si>
+  <si>
     <t>Caster Dualchip</t>
   </si>
   <si>
-    <t>Coagulating Gel</t>
+    <t>Guard Dualchip</t>
+  </si>
+  <si>
+    <t>Sniper Dualchip</t>
+  </si>
+  <si>
+    <t>Defender Dualchip</t>
+  </si>
+  <si>
+    <t>Specialist Dualchip</t>
+  </si>
+  <si>
+    <t>Medic Dualchip</t>
+  </si>
+  <si>
+    <t>Vanguard Dualchip</t>
+  </si>
+  <si>
+    <t>Supporter Dualchip</t>
+  </si>
+  <si>
+    <t>Cutting Stock Solution</t>
   </si>
   <si>
     <t>Compound Cutting Fluid</t>
-  </si>
-  <si>
-    <t>Crystalline Circuit</t>
-  </si>
-  <si>
-    <t>Crystalline Component</t>
-  </si>
-  <si>
-    <t>Crystalline Electroassembly</t>
-  </si>
-  <si>
-    <t>Cutting Stock Solution</t>
-  </si>
-  <si>
-    <t>D32 Steel</t>
-  </si>
-  <si>
-    <t>Damaged Device</t>
-  </si>
-  <si>
-    <t>Defender Chip</t>
-  </si>
-  <si>
-    <t>Defender Chip Pack</t>
-  </si>
-  <si>
-    <t>Defender Dualchip</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Diketon</t>
-  </si>
-  <si>
-    <t>Ester</t>
-  </si>
-  <si>
-    <t>Grindstone</t>
-  </si>
-  <si>
-    <t>Grindstone Pentahydrate</t>
-  </si>
-  <si>
-    <t>Guard Chip</t>
-  </si>
-  <si>
-    <t>Guard Chip Pack</t>
-  </si>
-  <si>
-    <t>Guard Dualchip</t>
-  </si>
-  <si>
-    <t>Incandescent Alloy</t>
-  </si>
-  <si>
-    <t>Incandescent Alloy Block</t>
-  </si>
-  <si>
-    <t>Integrated Device</t>
-  </si>
-  <si>
-    <t>Keton Colloid</t>
-  </si>
-  <si>
-    <t>Loxic Kohl</t>
-  </si>
-  <si>
-    <t>Manganese Ore</t>
-  </si>
-  <si>
-    <t>Manganese Trihydrate</t>
-  </si>
-  <si>
-    <t>Medic Chip</t>
-  </si>
-  <si>
-    <t>Medic Chip Pack</t>
-  </si>
-  <si>
-    <t>Medic Dualchip</t>
-  </si>
-  <si>
-    <t>Optimized Device</t>
-  </si>
-  <si>
-    <t>Orirock</t>
-  </si>
-  <si>
-    <t>Orirock Cluster</t>
-  </si>
-  <si>
-    <t>Orirock Concentration</t>
-  </si>
-  <si>
-    <t>Orirock Cube</t>
-  </si>
-  <si>
-    <t>Oriron</t>
-  </si>
-  <si>
-    <t>Oriron Block</t>
-  </si>
-  <si>
-    <t>Oriron Cluster</t>
-  </si>
-  <si>
-    <t>Oriron Shard</t>
-  </si>
-  <si>
-    <t>Polyester</t>
-  </si>
-  <si>
-    <t>Polyester Lump</t>
-  </si>
-  <si>
-    <t>Polyester Pack</t>
-  </si>
-  <si>
-    <t>Polyketon</t>
-  </si>
-  <si>
-    <t>Polymerization Preparation</t>
-  </si>
-  <si>
-    <t>Polymerized Gel</t>
-  </si>
-  <si>
-    <t>RMA70-12</t>
-  </si>
-  <si>
-    <t>RMA70-24</t>
-  </si>
-  <si>
-    <t>Refined Solvent</t>
-  </si>
-  <si>
-    <t>Semi-natural Solvent</t>
-  </si>
-  <si>
-    <t>Skill Summary - 1</t>
-  </si>
-  <si>
-    <t>Skill Summary - 2</t>
-  </si>
-  <si>
-    <t>Skill Summary - 3</t>
-  </si>
-  <si>
-    <t>Sniper Chip</t>
-  </si>
-  <si>
-    <t>Sniper Chip Pack</t>
-  </si>
-  <si>
-    <t>Sniper Dualchip</t>
-  </si>
-  <si>
-    <t>Specialist Chip</t>
-  </si>
-  <si>
-    <t>Specialist Chip Pack</t>
-  </si>
-  <si>
-    <t>Specialist Dualchip</t>
-  </si>
-  <si>
-    <t>Sugar</t>
-  </si>
-  <si>
-    <t>Sugar Lump</t>
-  </si>
-  <si>
-    <t>Sugar Pack</t>
-  </si>
-  <si>
-    <t>Sugar Substitute</t>
-  </si>
-  <si>
-    <t>Supporter Chip</t>
-  </si>
-  <si>
-    <t>Supporter Chip Pack</t>
-  </si>
-  <si>
-    <t>Supporter Dualchip</t>
-  </si>
-  <si>
-    <t>Vanguard Chip</t>
-  </si>
-  <si>
-    <t>Vanguard Chip Pack</t>
-  </si>
-  <si>
-    <t>Vanguard Dualchip</t>
-  </si>
-  <si>
-    <t>White Horse Kohl</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
     <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1"/>
   </cols>
@@ -656,25 +656,25 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>643</v>
+        <v>1390</v>
       </c>
       <c r="F2">
-        <v>206</v>
+        <v>1258</v>
       </c>
       <c r="G2">
-        <v>437</v>
+        <v>132</v>
       </c>
       <c r="H2" s="1">
-        <v>0.3204</v>
+        <v>0.905</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -682,25 +682,25 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>634</v>
+        <v>277</v>
       </c>
       <c r="F3">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="G3">
-        <v>598</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1">
-        <v>0.0568</v>
+        <v>0.8917</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -708,25 +708,25 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>93</v>
+        <v>3135</v>
       </c>
       <c r="F4">
-        <v>85</v>
+        <v>2382</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>753</v>
       </c>
       <c r="H4" s="1">
-        <v>0.914</v>
+        <v>0.7598</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -734,25 +734,25 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>25</v>
+        <v>481</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>406</v>
       </c>
       <c r="G5">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>0.8441</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -760,25 +760,25 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>61</v>
+        <v>485</v>
       </c>
       <c r="F6">
-        <v>22</v>
+        <v>421</v>
       </c>
       <c r="G6">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1">
-        <v>0.3607</v>
+        <v>0.868</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -795,33 +795,42 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>271</v>
+        <v>457</v>
       </c>
       <c r="F7">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="G7">
-        <v>195</v>
+        <v>355</v>
       </c>
       <c r="H7" s="1">
-        <v>0.2804</v>
+        <v>0.2232</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
       <c r="E8">
-        <v>13</v>
+        <v>10638</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>973</v>
       </c>
       <c r="G8">
-        <v>13</v>
+        <v>9665</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>0.0915</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -829,385 +838,394 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>112</v>
+        <v>776</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>234</v>
       </c>
       <c r="G9">
-        <v>112</v>
+        <v>542</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>0.3015</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>40</v>
+        <v>25470000</v>
       </c>
       <c r="F10">
-        <v>17</v>
+        <v>9800000</v>
       </c>
       <c r="G10">
-        <v>23</v>
+        <v>15670000</v>
       </c>
       <c r="H10" s="1">
-        <v>0.425</v>
+        <v>0.3848</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="F11">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="G11">
-        <v>140</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1">
-        <v>0.0789</v>
+        <v>0.9176</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>344</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>0.8171</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>554</v>
+        <v>317</v>
       </c>
       <c r="F13">
-        <v>40</v>
+        <v>257</v>
       </c>
       <c r="G13">
-        <v>514</v>
+        <v>60</v>
       </c>
       <c r="H13" s="1">
-        <v>0.0722</v>
+        <v>0.8107</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>136</v>
+        <v>287</v>
       </c>
       <c r="F14">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="G14">
-        <v>14</v>
+        <v>198</v>
       </c>
       <c r="H14" s="1">
-        <v>0.8971</v>
+        <v>0.3101</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>85</v>
+        <v>479</v>
       </c>
       <c r="F15">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>316</v>
       </c>
       <c r="H15" s="1">
-        <v>0.9529</v>
+        <v>0.3403</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>25</v>
+        <v>167</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="G16">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>0.8922</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>54</v>
+        <v>693</v>
       </c>
       <c r="F17">
-        <v>20</v>
+        <v>567</v>
       </c>
       <c r="G17">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="H17" s="1">
-        <v>0.3704</v>
+        <v>0.8182</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>317</v>
+        <v>533</v>
       </c>
       <c r="F18">
-        <v>257</v>
+        <v>124</v>
       </c>
       <c r="G18">
-        <v>60</v>
+        <v>409</v>
       </c>
       <c r="H18" s="1">
-        <v>0.8107</v>
+        <v>0.2326</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>167</v>
+        <v>550</v>
       </c>
       <c r="F19">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="G19">
-        <v>18</v>
+        <v>426</v>
       </c>
       <c r="H19" s="1">
-        <v>0.8922</v>
+        <v>0.2255</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>211</v>
+        <v>696</v>
       </c>
       <c r="F20">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="G20">
-        <v>17</v>
+        <v>480</v>
       </c>
       <c r="H20" s="1">
-        <v>0.9194</v>
+        <v>0.3103</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>550</v>
+        <v>211</v>
       </c>
       <c r="F21">
-        <v>124</v>
+        <v>194</v>
       </c>
       <c r="G21">
-        <v>426</v>
+        <v>17</v>
       </c>
       <c r="H21" s="1">
-        <v>0.2255</v>
+        <v>0.9194</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>706</v>
+        <v>440</v>
       </c>
       <c r="F22">
-        <v>22</v>
+        <v>373</v>
       </c>
       <c r="G22">
-        <v>684</v>
+        <v>67</v>
       </c>
       <c r="H22" s="1">
-        <v>0.0312</v>
+        <v>0.8477</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>150</v>
+        <v>643</v>
       </c>
       <c r="F23">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="G23">
-        <v>17</v>
+        <v>437</v>
       </c>
       <c r="H23" s="1">
-        <v>0.8867</v>
+        <v>0.3204</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1219,99 +1237,99 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>55</v>
+        <v>306</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="G24">
-        <v>50</v>
+        <v>226</v>
       </c>
       <c r="H24" s="1">
-        <v>0.09089999999999999</v>
+        <v>0.2614</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="D25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>90</v>
+        <v>136</v>
       </c>
       <c r="F25">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="G25">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="H25" s="1">
-        <v>0.3</v>
+        <v>0.8971</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="F26">
-        <v>53</v>
+        <v>184</v>
       </c>
       <c r="G26">
-        <v>144</v>
+        <v>23</v>
       </c>
       <c r="H26" s="1">
-        <v>0.269</v>
+        <v>0.8889</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="F27">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="G27">
-        <v>425</v>
+        <v>326</v>
       </c>
       <c r="H27" s="1">
-        <v>0.0513</v>
+        <v>0.2658</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1323,68 +1341,68 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <v>444</v>
+        <v>271</v>
       </c>
       <c r="F28">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="G28">
-        <v>326</v>
+        <v>195</v>
       </c>
       <c r="H28" s="1">
-        <v>0.2658</v>
+        <v>0.2804</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>661</v>
+        <v>112</v>
       </c>
       <c r="F29">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="G29">
-        <v>614</v>
+        <v>10</v>
       </c>
       <c r="H29" s="1">
-        <v>0.0711</v>
+        <v>0.9107</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
       </c>
       <c r="E30">
-        <v>25470000</v>
+        <v>40</v>
       </c>
       <c r="F30">
-        <v>9800000</v>
+        <v>10</v>
       </c>
       <c r="G30">
-        <v>15670000</v>
+        <v>30</v>
       </c>
       <c r="H30" s="1">
-        <v>0.3848</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1392,25 +1410,25 @@
         <v>36</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>696</v>
+        <v>706</v>
       </c>
       <c r="F31">
-        <v>216</v>
+        <v>22</v>
       </c>
       <c r="G31">
-        <v>480</v>
+        <v>684</v>
       </c>
       <c r="H31" s="1">
-        <v>0.3103</v>
+        <v>0.0312</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1418,25 +1436,25 @@
         <v>37</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>533</v>
+        <v>661</v>
       </c>
       <c r="F32">
-        <v>124</v>
+        <v>47</v>
       </c>
       <c r="G32">
-        <v>409</v>
+        <v>614</v>
       </c>
       <c r="H32" s="1">
-        <v>0.2326</v>
+        <v>0.0711</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1453,16 +1471,16 @@
         <v>1</v>
       </c>
       <c r="E33">
-        <v>634</v>
+        <v>537</v>
       </c>
       <c r="F33">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G33">
-        <v>608</v>
+        <v>517</v>
       </c>
       <c r="H33" s="1">
-        <v>0.041</v>
+        <v>0.0372</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1470,25 +1488,25 @@
         <v>39</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C34">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="D34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>66</v>
+        <v>634</v>
       </c>
       <c r="F34">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="G34">
-        <v>4</v>
+        <v>598</v>
       </c>
       <c r="H34" s="1">
-        <v>0.9394</v>
+        <v>0.0568</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1496,25 +1514,25 @@
         <v>40</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>25</v>
+        <v>725</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G35">
-        <v>20</v>
+        <v>697</v>
       </c>
       <c r="H35" s="1">
-        <v>0.2</v>
+        <v>0.0386</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1528,19 +1546,19 @@
         <v>300</v>
       </c>
       <c r="D36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>39</v>
+        <v>448</v>
       </c>
       <c r="F36">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G36">
-        <v>25</v>
+        <v>425</v>
       </c>
       <c r="H36" s="1">
-        <v>0.359</v>
+        <v>0.0513</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1557,16 +1575,16 @@
         <v>1</v>
       </c>
       <c r="E37">
-        <v>471</v>
+        <v>632</v>
       </c>
       <c r="F37">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G37">
-        <v>442</v>
+        <v>612</v>
       </c>
       <c r="H37" s="1">
-        <v>0.0616</v>
+        <v>0.0316</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1574,25 +1592,25 @@
         <v>43</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
       </c>
       <c r="E38">
-        <v>277</v>
+        <v>746</v>
       </c>
       <c r="F38">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="G38">
-        <v>30</v>
+        <v>701</v>
       </c>
       <c r="H38" s="1">
-        <v>0.8917</v>
+        <v>0.0603</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1609,16 +1627,16 @@
         <v>1</v>
       </c>
       <c r="E39">
-        <v>776</v>
+        <v>197</v>
       </c>
       <c r="F39">
-        <v>234</v>
+        <v>53</v>
       </c>
       <c r="G39">
-        <v>542</v>
+        <v>144</v>
       </c>
       <c r="H39" s="1">
-        <v>0.3015</v>
+        <v>0.269</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1635,16 +1653,16 @@
         <v>1</v>
       </c>
       <c r="E40">
-        <v>746</v>
+        <v>634</v>
       </c>
       <c r="F40">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="G40">
-        <v>701</v>
+        <v>608</v>
       </c>
       <c r="H40" s="1">
-        <v>0.0603</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1652,25 +1670,25 @@
         <v>46</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C41">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="D41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>693</v>
+        <v>552</v>
       </c>
       <c r="F41">
-        <v>567</v>
+        <v>44</v>
       </c>
       <c r="G41">
-        <v>126</v>
+        <v>508</v>
       </c>
       <c r="H41" s="1">
-        <v>0.8182</v>
+        <v>0.07969999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1678,25 +1696,25 @@
         <v>47</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C42">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="D42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>440</v>
+        <v>554</v>
       </c>
       <c r="F42">
-        <v>373</v>
+        <v>40</v>
       </c>
       <c r="G42">
-        <v>67</v>
+        <v>514</v>
       </c>
       <c r="H42" s="1">
-        <v>0.8477</v>
+        <v>0.0722</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1730,25 +1748,25 @@
         <v>49</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>479</v>
+        <v>150</v>
       </c>
       <c r="F44">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="G44">
-        <v>316</v>
+        <v>17</v>
       </c>
       <c r="H44" s="1">
-        <v>0.3403</v>
+        <v>0.8867</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1756,25 +1774,25 @@
         <v>50</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
       </c>
       <c r="E45">
-        <v>170</v>
+        <v>55</v>
       </c>
       <c r="F45">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="G45">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="H45" s="1">
-        <v>0.9176</v>
+        <v>0.09089999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1791,16 +1809,16 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <v>485</v>
+        <v>59</v>
       </c>
       <c r="F46">
-        <v>421</v>
+        <v>54</v>
       </c>
       <c r="G46">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="H46" s="1">
-        <v>0.868</v>
+        <v>0.9153</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1808,25 +1826,25 @@
         <v>52</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
       </c>
       <c r="E47">
-        <v>355</v>
+        <v>25</v>
       </c>
       <c r="F47">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G47">
-        <v>336</v>
+        <v>15</v>
       </c>
       <c r="H47" s="1">
-        <v>0.0535</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1834,25 +1852,25 @@
         <v>53</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C48">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>287</v>
+        <v>152</v>
       </c>
       <c r="F48">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="G48">
-        <v>198</v>
+        <v>140</v>
       </c>
       <c r="H48" s="1">
-        <v>0.3101</v>
+        <v>0.0789</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1869,16 +1887,16 @@
         <v>1</v>
       </c>
       <c r="E49">
-        <v>421</v>
+        <v>85</v>
       </c>
       <c r="F49">
-        <v>344</v>
+        <v>81</v>
       </c>
       <c r="G49">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="H49" s="1">
-        <v>0.8171</v>
+        <v>0.9529</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1886,25 +1904,25 @@
         <v>55</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C50">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>552</v>
+        <v>25</v>
       </c>
       <c r="F50">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>508</v>
+        <v>25</v>
       </c>
       <c r="H50" s="1">
-        <v>0.07969999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1921,16 +1939,16 @@
         <v>1</v>
       </c>
       <c r="E51">
-        <v>537</v>
+        <v>471</v>
       </c>
       <c r="F51">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G51">
-        <v>517</v>
+        <v>442</v>
       </c>
       <c r="H51" s="1">
-        <v>0.0372</v>
+        <v>0.0616</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1938,25 +1956,25 @@
         <v>57</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
       </c>
       <c r="E52">
-        <v>457</v>
+        <v>93</v>
       </c>
       <c r="F52">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="G52">
-        <v>355</v>
+        <v>8</v>
       </c>
       <c r="H52" s="1">
-        <v>0.2232</v>
+        <v>0.914</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1964,59 +1982,77 @@
         <v>58</v>
       </c>
       <c r="B53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
       </c>
       <c r="E53">
-        <v>632</v>
+        <v>25</v>
       </c>
       <c r="F53">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G53">
-        <v>612</v>
+        <v>25</v>
       </c>
       <c r="H53" s="1">
-        <v>0.0316</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>59</v>
       </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>300</v>
+      </c>
+      <c r="D54" t="b">
+        <v>1</v>
+      </c>
       <c r="E54">
-        <v>32</v>
+        <v>355</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G54">
-        <v>32</v>
+        <v>336</v>
       </c>
       <c r="H54" s="1">
-        <v>0</v>
+        <v>0.0535</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>60</v>
       </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>300</v>
+      </c>
+      <c r="D55" t="b">
+        <v>1</v>
+      </c>
       <c r="E55">
-        <v>34</v>
+        <v>350</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G55">
-        <v>34</v>
+        <v>340</v>
       </c>
       <c r="H55" s="1">
-        <v>0</v>
+        <v>0.0286</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2027,22 +2063,22 @@
         <v>2</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56">
-        <v>1390</v>
+        <v>64</v>
       </c>
       <c r="F56">
-        <v>1258</v>
+        <v>61</v>
       </c>
       <c r="G56">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="H56" s="1">
-        <v>0.905</v>
+        <v>0.9530999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2053,22 +2089,22 @@
         <v>3</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>3135</v>
+        <v>20</v>
       </c>
       <c r="F57">
-        <v>2382</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>753</v>
+        <v>20</v>
       </c>
       <c r="H57" s="1">
-        <v>0.7598</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2076,25 +2112,25 @@
         <v>63</v>
       </c>
       <c r="B58">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>10638</v>
+        <v>88</v>
       </c>
       <c r="F58">
-        <v>973</v>
+        <v>71</v>
       </c>
       <c r="G58">
-        <v>9665</v>
+        <v>17</v>
       </c>
       <c r="H58" s="1">
-        <v>0.0915</v>
+        <v>0.8068</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2102,25 +2138,25 @@
         <v>64</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C59">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
       </c>
       <c r="E59">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="F59">
-        <v>102</v>
+        <v>5</v>
       </c>
       <c r="G59">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H59" s="1">
-        <v>0.9107</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2128,25 +2164,25 @@
         <v>65</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
       </c>
       <c r="E60">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F60">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="G60">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="H60" s="1">
-        <v>0.25</v>
+        <v>0.9394</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2154,25 +2190,25 @@
         <v>66</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="F61">
+        <v>5</v>
+      </c>
+      <c r="G61">
         <v>20</v>
       </c>
-      <c r="G61">
-        <v>48</v>
-      </c>
       <c r="H61" s="1">
-        <v>0.2941</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2180,25 +2216,25 @@
         <v>67</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
       </c>
       <c r="E62">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="F62">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="G62">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H62" s="1">
-        <v>0.8068</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2206,77 +2242,59 @@
         <v>68</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C63">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
       </c>
       <c r="E63">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="F63">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G63">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="H63" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>69</v>
       </c>
-      <c r="B64">
-        <v>4</v>
-      </c>
-      <c r="C64">
-        <v>300</v>
-      </c>
-      <c r="D64" t="b">
-        <v>0</v>
-      </c>
       <c r="E64">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="F64">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G64">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="H64" s="1">
-        <v>0.1429</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>70</v>
       </c>
-      <c r="B65">
-        <v>2</v>
-      </c>
-      <c r="C65">
-        <v>100</v>
-      </c>
-      <c r="D65" t="b">
-        <v>1</v>
-      </c>
       <c r="E65">
-        <v>481</v>
+        <v>32</v>
       </c>
       <c r="F65">
-        <v>406</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="H65" s="1">
-        <v>0.8441</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2290,19 +2308,19 @@
         <v>300</v>
       </c>
       <c r="D66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>350</v>
+        <v>61</v>
       </c>
       <c r="F66">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G66">
-        <v>340</v>
+        <v>39</v>
       </c>
       <c r="H66" s="1">
-        <v>0.0286</v>
+        <v>0.3607</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2310,25 +2328,25 @@
         <v>72</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C67">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>306</v>
+        <v>90</v>
       </c>
       <c r="F67">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="G67">
-        <v>226</v>
+        <v>63</v>
       </c>
       <c r="H67" s="1">
-        <v>0.2614</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2336,25 +2354,25 @@
         <v>73</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68">
-        <v>207</v>
+        <v>68</v>
       </c>
       <c r="F68">
-        <v>184</v>
+        <v>20</v>
       </c>
       <c r="G68">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="H68" s="1">
-        <v>0.8889</v>
+        <v>0.2941</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2362,25 +2380,25 @@
         <v>74</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C69">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F69">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="G69">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H69" s="1">
-        <v>0.9530999999999999</v>
+        <v>0.3704</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2388,25 +2406,25 @@
         <v>75</v>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C70">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G70">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="H70" s="1">
-        <v>0</v>
+        <v>0.1429</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2423,16 +2441,16 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F71">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G71">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H71" s="1">
-        <v>0.2</v>
+        <v>0.359</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2440,25 +2458,25 @@
         <v>77</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C72">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="F72">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="G72">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="H72" s="1">
-        <v>0.9153</v>
+        <v>0.3235</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2466,77 +2484,59 @@
         <v>78</v>
       </c>
       <c r="B73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C73">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F73">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G73">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H73" s="1">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>79</v>
       </c>
-      <c r="B74">
-        <v>4</v>
-      </c>
-      <c r="C74">
-        <v>300</v>
-      </c>
-      <c r="D74" t="b">
-        <v>0</v>
-      </c>
       <c r="E74">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F74">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G74">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H74" s="1">
-        <v>0.3235</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>80</v>
       </c>
-      <c r="B75">
-        <v>4</v>
-      </c>
-      <c r="C75">
-        <v>300</v>
-      </c>
-      <c r="D75" t="b">
-        <v>1</v>
-      </c>
       <c r="E75">
-        <v>725</v>
+        <v>13</v>
       </c>
       <c r="F75">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>697</v>
+        <v>13</v>
       </c>
       <c r="H75" s="1">
-        <v>0.0386</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:8">

</xml_diff>

<commit_message>
main.py: corrected mastery resource calc
</commit_message>
<xml_diff>
--- a/files/reports/2021-10-27/resources-report.xlsx
+++ b/files/reports/2021-10-27/resources-report.xlsx
@@ -798,13 +798,13 @@
         <v>457</v>
       </c>
       <c r="F7">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="G7">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="H7" s="1">
-        <v>0.2232</v>
+        <v>0.2473</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -824,13 +824,13 @@
         <v>10638</v>
       </c>
       <c r="F8">
-        <v>973</v>
+        <v>1453</v>
       </c>
       <c r="G8">
-        <v>9665</v>
+        <v>9185</v>
       </c>
       <c r="H8" s="1">
-        <v>0.0915</v>
+        <v>0.1366</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -850,13 +850,13 @@
         <v>776</v>
       </c>
       <c r="F9">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="G9">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="H9" s="1">
-        <v>0.3015</v>
+        <v>0.3119</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1006,13 +1006,13 @@
         <v>479</v>
       </c>
       <c r="F15">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G15">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H15" s="1">
-        <v>0.3403</v>
+        <v>0.3486</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1084,13 +1084,13 @@
         <v>533</v>
       </c>
       <c r="F18">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="G18">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="H18" s="1">
-        <v>0.2326</v>
+        <v>0.2608</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1110,13 +1110,13 @@
         <v>550</v>
       </c>
       <c r="F19">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="G19">
-        <v>426</v>
+        <v>405</v>
       </c>
       <c r="H19" s="1">
-        <v>0.2255</v>
+        <v>0.2636</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1136,13 +1136,13 @@
         <v>696</v>
       </c>
       <c r="F20">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="G20">
-        <v>480</v>
+        <v>448</v>
       </c>
       <c r="H20" s="1">
-        <v>0.3103</v>
+        <v>0.3563</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1214,13 +1214,13 @@
         <v>643</v>
       </c>
       <c r="F23">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="G23">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="H23" s="1">
-        <v>0.3204</v>
+        <v>0.3406</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1318,13 +1318,13 @@
         <v>444</v>
       </c>
       <c r="F27">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G27">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="H27" s="1">
-        <v>0.2658</v>
+        <v>0.2748</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1422,13 +1422,13 @@
         <v>706</v>
       </c>
       <c r="F31">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="G31">
-        <v>684</v>
+        <v>644</v>
       </c>
       <c r="H31" s="1">
-        <v>0.0312</v>
+        <v>0.0878</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1448,13 +1448,13 @@
         <v>661</v>
       </c>
       <c r="F32">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G32">
-        <v>614</v>
+        <v>583</v>
       </c>
       <c r="H32" s="1">
-        <v>0.0711</v>
+        <v>0.118</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1474,13 +1474,13 @@
         <v>537</v>
       </c>
       <c r="F33">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G33">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="H33" s="1">
-        <v>0.0372</v>
+        <v>0.0726</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1500,13 +1500,13 @@
         <v>634</v>
       </c>
       <c r="F34">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="G34">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="H34" s="1">
-        <v>0.0568</v>
+        <v>0.0978</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1526,13 +1526,13 @@
         <v>725</v>
       </c>
       <c r="F35">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="G35">
-        <v>697</v>
+        <v>660</v>
       </c>
       <c r="H35" s="1">
-        <v>0.0386</v>
+        <v>0.0897</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1552,13 +1552,13 @@
         <v>448</v>
       </c>
       <c r="F36">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="G36">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="H36" s="1">
-        <v>0.0513</v>
+        <v>0.0781</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1578,13 +1578,13 @@
         <v>632</v>
       </c>
       <c r="F37">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="G37">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="H37" s="1">
-        <v>0.0316</v>
+        <v>0.0839</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1604,13 +1604,13 @@
         <v>746</v>
       </c>
       <c r="F38">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="G38">
-        <v>701</v>
+        <v>658</v>
       </c>
       <c r="H38" s="1">
-        <v>0.0603</v>
+        <v>0.118</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1656,13 +1656,13 @@
         <v>634</v>
       </c>
       <c r="F40">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G40">
-        <v>608</v>
+        <v>593</v>
       </c>
       <c r="H40" s="1">
-        <v>0.041</v>
+        <v>0.06469999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1682,13 +1682,13 @@
         <v>552</v>
       </c>
       <c r="F41">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="G41">
-        <v>508</v>
+        <v>486</v>
       </c>
       <c r="H41" s="1">
-        <v>0.07969999999999999</v>
+        <v>0.1196</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1708,13 +1708,13 @@
         <v>554</v>
       </c>
       <c r="F42">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="G42">
-        <v>514</v>
+        <v>484</v>
       </c>
       <c r="H42" s="1">
-        <v>0.0722</v>
+        <v>0.1264</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1734,13 +1734,13 @@
         <v>612</v>
       </c>
       <c r="F43">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="G43">
-        <v>583</v>
+        <v>557</v>
       </c>
       <c r="H43" s="1">
-        <v>0.0474</v>
+        <v>0.08989999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1942,13 +1942,13 @@
         <v>471</v>
       </c>
       <c r="F51">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G51">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="H51" s="1">
-        <v>0.0616</v>
+        <v>0.0743</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2020,13 +2020,13 @@
         <v>355</v>
       </c>
       <c r="F54">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="G54">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="H54" s="1">
-        <v>0.0535</v>
+        <v>0.1099</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2046,13 +2046,13 @@
         <v>350</v>
       </c>
       <c r="F55">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="G55">
-        <v>340</v>
+        <v>312</v>
       </c>
       <c r="H55" s="1">
-        <v>0.0286</v>
+        <v>0.1086</v>
       </c>
     </row>
     <row r="56" spans="1:8">

</xml_diff>